<commit_message>
cluster analysis adjusted pca
used 7 PC's according to the cpv plot
</commit_message>
<xml_diff>
--- a/_CLUSTER/groups_time_area/PCA/control_points_count.xlsx
+++ b/_CLUSTER/groups_time_area/PCA/control_points_count.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -376,7 +376,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1669</v>
+        <v>2106</v>
       </c>
     </row>
     <row r="3">
@@ -384,23 +384,15 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>956</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>846</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B5" t="n">
-        <v>787</v>
+        <v>544</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cluster analyss Fe-number Frost
-didn't include the SiO2, only the 2 variables
-clear difference between area1 and rest of areas
</commit_message>
<xml_diff>
--- a/_CLUSTER/groups_time_area/PCA/control_points_count.xlsx
+++ b/_CLUSTER/groups_time_area/PCA/control_points_count.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -376,7 +376,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>2106</v>
+        <v>2152</v>
       </c>
     </row>
     <row r="3">
@@ -384,15 +384,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>1608</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>544</v>
+        <v>2106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>